<commit_message>
new update at 1.7
</commit_message>
<xml_diff>
--- a/预算.xlsx
+++ b/预算.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="115">
   <si>
     <t>航班号</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -500,15 +500,27 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>hmx+Daniel</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>我给倍子221。Daniel给倍子413。倍子给Sophy383.5。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Sophy给我461.Daniel给我250</t>
+    <t>HMX+D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>XX应该</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从XX处收取</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>合并版本</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>共计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>原始版本</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -520,7 +532,7 @@
     <numFmt numFmtId="176" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     <numFmt numFmtId="177" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -587,6 +599,20 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="微软雅黑"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -644,7 +670,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -711,6 +737,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -728,6 +757,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2476,7 +2517,7 @@
       <c r="I2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="24">
+      <c r="J2" s="25">
         <v>2679</v>
       </c>
       <c r="K2" s="1"/>
@@ -2513,7 +2554,7 @@
       <c r="I3" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="24"/>
+      <c r="J3" s="25"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -2548,7 +2589,7 @@
       <c r="I4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="24">
+      <c r="J4" s="25">
         <v>2796</v>
       </c>
       <c r="K4" s="1"/>
@@ -2585,7 +2626,7 @@
       <c r="I5" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="J5" s="24"/>
+      <c r="J5" s="25"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -2620,7 +2661,7 @@
       <c r="I6" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="25"/>
+      <c r="J6" s="26"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -3082,7 +3123,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3107,10 +3148,10 @@
       <c r="A2" s="16">
         <v>42750</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="26">
+      <c r="C2" s="27">
         <v>1680</v>
       </c>
     </row>
@@ -3118,15 +3159,15 @@
       <c r="A3" s="16">
         <v>42751</v>
       </c>
-      <c r="B3" s="26"/>
-      <c r="C3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="27"/>
     </row>
     <row r="4" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16">
         <v>42752</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
     </row>
     <row r="5" spans="1:3" ht="49.5" x14ac:dyDescent="0.3">
       <c r="A5" s="16">
@@ -3143,10 +3184,10 @@
       <c r="A6" s="16">
         <v>42754</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="27">
         <v>890</v>
       </c>
     </row>
@@ -3154,15 +3195,15 @@
       <c r="A7" s="16">
         <v>42755</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="16">
         <v>42756</v>
       </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="16">
@@ -3180,10 +3221,10 @@
       <c r="A11" s="16">
         <v>42759</v>
       </c>
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="27">
         <v>1000</v>
       </c>
     </row>
@@ -3191,8 +3232,8 @@
       <c r="A12" s="16">
         <v>42760</v>
       </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="16">
@@ -3202,7 +3243,7 @@
         <v>100</v>
       </c>
       <c r="C13" s="20">
-        <v>0</v>
+        <v>-389</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -3241,7 +3282,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3535,7 +3576,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3565,9 +3606,9 @@
         <f>国际机票!J2+国际机票!J4</f>
         <v>5475</v>
       </c>
-      <c r="C2" s="27">
+      <c r="C2" s="28">
         <f>SUM(B2:B9)</f>
-        <v>9340.4833333333336</v>
+        <v>9210.8166666666657</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -3578,17 +3619,17 @@
         <f>7.4*SUM(欧洲交通!I2:I6)/4</f>
         <v>721.5</v>
       </c>
-      <c r="C3" s="28"/>
+      <c r="C3" s="29"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="11">
-        <f>(SUM(住宿!C2:C8)+住宿!C13)/3+住宿!C11/4</f>
-        <v>1258.3333333333335</v>
-      </c>
-      <c r="C4" s="28"/>
+        <f>(SUM(住宿!C2:'住宿'!C8)+住宿!C13)/3+住宿!C11/4</f>
+        <v>1128.6666666666665</v>
+      </c>
+      <c r="C4" s="29"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="12" t="s">
@@ -3598,7 +3639,7 @@
         <f>SUM(签证!B2:B14)</f>
         <v>1132</v>
       </c>
-      <c r="C5" s="28"/>
+      <c r="C5" s="29"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="12" t="s">
@@ -3607,7 +3648,7 @@
       <c r="B6" s="12">
         <v>175</v>
       </c>
-      <c r="C6" s="28"/>
+      <c r="C6" s="29"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="12" t="s">
@@ -3617,7 +3658,7 @@
         <f>(20+15)*7.32/2</f>
         <v>128.1</v>
       </c>
-      <c r="C7" s="28"/>
+      <c r="C7" s="29"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="12" t="s">
@@ -3627,12 +3668,12 @@
         <f>SUM(体验门票等!C1:'体验门票等'!C30)</f>
         <v>450.55</v>
       </c>
-      <c r="C8" s="28"/>
+      <c r="C8" s="29"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="12"/>
       <c r="B9" s="12"/>
-      <c r="C9" s="28"/>
+      <c r="C9" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3649,231 +3690,315 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="6" max="6" width="9.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A1" s="23"/>
-      <c r="B1" s="29" t="s">
+    <row r="1" spans="1:7" ht="22.5" x14ac:dyDescent="0.4">
+      <c r="A1" s="34" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+    </row>
+    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A2" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A2" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="30"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D3" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E3" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="23" t="s">
+      <c r="F3" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="29"/>
-      <c r="B3" s="23" t="s">
+      <c r="G3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A4" s="30"/>
+      <c r="B4" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23">
-        <f>455/3</f>
-        <v>151.66666666666666</v>
-      </c>
-      <c r="E3" s="23">
+      <c r="C4" s="23"/>
+      <c r="D4" s="23">
+        <f>(455+住宿!C13)/3</f>
+        <v>22</v>
+      </c>
+      <c r="E4" s="23">
         <f>总表!B4</f>
-        <v>1258.3333333333335</v>
-      </c>
-      <c r="F3" s="23">
+        <v>1128.6666666666665</v>
+      </c>
+      <c r="F4" s="23">
         <f>住宿!C11/4</f>
         <v>250</v>
       </c>
-      <c r="G3" s="5"/>
-    </row>
-    <row r="4" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="29"/>
-      <c r="B4" s="23" t="s">
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A5" s="30"/>
+      <c r="B5" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="23">
-        <f>51*B6</f>
-        <v>372.81</v>
-      </c>
-      <c r="D4" s="23"/>
-      <c r="E4" s="23">
-        <f>56.5*B6</f>
-        <v>413.01499999999999</v>
-      </c>
-      <c r="F4" s="23">
-        <f>56.5*B6</f>
-        <v>413.01499999999999</v>
-      </c>
-      <c r="G4" s="5"/>
-    </row>
-    <row r="5" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="29"/>
-      <c r="B5" s="23" t="s">
+      <c r="C5" s="23">
+        <f>55.75*B7</f>
+        <v>407.53249999999997</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23">
+        <f>62*B7+415</f>
+        <v>868.22</v>
+      </c>
+      <c r="F5" s="23">
+        <f>23*B7</f>
+        <v>168.13</v>
+      </c>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A6" s="30"/>
+      <c r="B6" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="C5" s="23">
-        <f>109*B6</f>
+      <c r="C6" s="23">
+        <f>109*B7</f>
         <v>796.79</v>
       </c>
-      <c r="D5" s="23">
-        <f>C5</f>
+      <c r="D6" s="23">
+        <f>C6</f>
         <v>796.79</v>
       </c>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="23" t="s">
+      <c r="E6" s="23"/>
+      <c r="F6" s="23">
+        <f>SUM(F4:F5)</f>
+        <v>418.13</v>
+      </c>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="23">
+      <c r="B7" s="23">
         <v>7.31</v>
       </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="5"/>
-    </row>
-    <row r="7" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="23"/>
-      <c r="B7" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
       <c r="F7" s="23"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="24"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="5"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="33" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="5"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A10" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="5"/>
+    </row>
+    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A11" s="30"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="F11" s="23"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A12" s="30"/>
+      <c r="B12" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23">
+        <v>22</v>
+      </c>
+      <c r="E12" s="23">
+        <f>E4+F4</f>
+        <v>1378.6666666666665</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="G12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A13" s="30"/>
+      <c r="B13" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="23">
+        <f>C5</f>
+        <v>407.53249999999997</v>
+      </c>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23">
+        <f>E5+F5</f>
+        <v>1036.3499999999999</v>
+      </c>
+      <c r="F13" s="23"/>
+      <c r="G13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A14" s="30"/>
+      <c r="B14" s="23" t="s">
+        <v>104</v>
+      </c>
+      <c r="C14" s="24">
+        <f>C6</f>
+        <v>796.79</v>
+      </c>
+      <c r="D14" s="24">
+        <f>C14</f>
+        <v>796.79</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+    </row>
+    <row r="15" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+    </row>
+    <row r="16" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="34" t="s">
+        <v>113</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+    </row>
+    <row r="17" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A17" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23" t="s">
+      <c r="B17" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+    </row>
+    <row r="18" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A18" s="30"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="D8" s="23" t="s">
+      <c r="D18" s="24" t="s">
         <v>103</v>
       </c>
-      <c r="E8" s="23" t="s">
+      <c r="E18" s="24" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A19" s="30"/>
+      <c r="B19" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24">
+        <f>E12-C14</f>
+        <v>581.87666666666655</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A20" s="30"/>
+      <c r="B20" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="24">
+        <f>C13-D12</f>
+        <v>385.53249999999997</v>
+      </c>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24">
+        <f>E13-D14</f>
+        <v>239.55999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="16.5" x14ac:dyDescent="0.15">
+      <c r="A21" s="30"/>
+      <c r="B21" s="24" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="29"/>
-      <c r="B9" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23">
-        <f>D3-C4</f>
-        <v>-221.14333333333335</v>
-      </c>
-      <c r="E9" s="23">
-        <f>E3-C5</f>
-        <v>461.54333333333352</v>
-      </c>
-      <c r="F9" s="23">
-        <f>住宿!C11/4</f>
-        <v>250</v>
-      </c>
-      <c r="G9" s="5">
-        <f>E9+F9</f>
-        <v>711.54333333333352</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A10" s="29"/>
-      <c r="B10" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="C10" s="23">
-        <f>C4-D3</f>
-        <v>221.14333333333335</v>
-      </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23">
-        <f>E4-D5</f>
-        <v>-383.77499999999998</v>
-      </c>
-      <c r="F10" s="23">
-        <f>F4</f>
-        <v>413.01499999999999</v>
-      </c>
-      <c r="G10" s="5">
-        <f>E10+F10</f>
-        <v>29.240000000000009</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="A11" s="29"/>
-      <c r="B11" s="23" t="s">
-        <v>104</v>
-      </c>
-      <c r="C11" s="23">
-        <f>C5-E3</f>
-        <v>-461.54333333333352</v>
-      </c>
-      <c r="D11" s="23">
-        <f>D5-E4</f>
-        <v>383.77499999999998</v>
-      </c>
-      <c r="E11" s="23"/>
-      <c r="F11" s="23">
-        <f>F9+F10</f>
-        <v>663.01499999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B12" s="23"/>
-    </row>
-    <row r="13" spans="1:7" ht="16.5" x14ac:dyDescent="0.15">
-      <c r="B13" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="E13" t="s">
-        <v>111</v>
-      </c>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="A8:A11"/>
+  <mergeCells count="9">
+    <mergeCell ref="A9:E9"/>
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:A6"/>
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A17:A21"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B10:E10"/>
+    <mergeCell ref="B17:E17"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>